<commit_message>
Updated FMA Days Paid
</commit_message>
<xml_diff>
--- a/analyses/monitoring_costs/FMA Days Paid.xlsx
+++ b/analyses/monitoring_costs/FMA Days Paid.xlsx
@@ -10,14 +10,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="qaiong0EBtPUWe55GGi5FXsyYAZuhQKHBCtsJJ/u90o="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="9Aub7KQy0WieWVTHoa8W3TspX4bRA1mWCuo5wWltqDg="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="64">
   <si>
     <t>Contract</t>
   </si>
@@ -137,6 +137,18 @@
   </si>
   <si>
     <t>Aug23Aug24</t>
+  </si>
+  <si>
+    <t>Aug23Sept24</t>
+  </si>
+  <si>
+    <t>Extended contract from 8/17/24 - 9/30/2024 added 350 new Guaranteed days</t>
+  </si>
+  <si>
+    <t>Aug23Sept 24</t>
+  </si>
+  <si>
+    <t>Extended contract from 8/17/24 - 9/30/2024</t>
   </si>
   <si>
     <t>Dates</t>
@@ -4082,6 +4094,9 @@
       <c r="C85" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D85" s="2">
+        <v>0.0</v>
+      </c>
       <c r="E85" s="2">
         <v>134.5</v>
       </c>
@@ -4588,9 +4603,95 @@
       <c r="C97" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
+      <c r="D97" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E97" s="2">
+        <v>138.0</v>
+      </c>
+      <c r="F97" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G97" s="2">
+        <v>101924.04</v>
+      </c>
+      <c r="H97" s="2">
+        <v>42634.88</v>
+      </c>
+      <c r="I97" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J97" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K97" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L97" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M97" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="98" ht="14.25" customHeight="1">
+      <c r="A98" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B98" s="2">
+        <v>2024.0</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D98" s="2">
+        <v>106.5</v>
+      </c>
+      <c r="E98" s="2">
+        <v>206.5</v>
+      </c>
+      <c r="F98" s="2">
+        <v>154028.82</v>
+      </c>
+      <c r="G98" s="2">
+        <v>152516.77</v>
+      </c>
+      <c r="H98" s="2">
+        <v>92274.89</v>
+      </c>
+      <c r="I98" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J98" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K98" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L98" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M98" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="N98" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="99" ht="14.25" customHeight="1">
+      <c r="A99" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B99" s="2">
+        <v>2024.0</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N99" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="100" ht="14.25" customHeight="1"/>
     <row r="101" ht="14.25" customHeight="1"/>
     <row r="102" ht="14.25" customHeight="1"/>
@@ -5529,25 +5630,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2">
@@ -5555,10 +5656,10 @@
         <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D2" s="13">
         <v>1151.54</v>
@@ -5575,10 +5676,10 @@
         <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D3" s="13">
         <v>1174.56</v>
@@ -5595,10 +5696,10 @@
         <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D4" s="15">
         <v>1198.02</v>
@@ -5615,10 +5716,10 @@
         <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D5" s="13">
         <v>1255.42</v>
@@ -5635,10 +5736,10 @@
         <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D6" s="13">
         <v>1289.32</v>
@@ -5661,10 +5762,10 @@
         <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D7" s="13">
         <v>1328.0</v>
@@ -5687,10 +5788,10 @@
         <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D8" s="13">
         <v>1370.5</v>
@@ -5713,10 +5814,10 @@
         <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D9" s="13">
         <v>1417.7</v>

</xml_diff>

<commit_message>
Updated FMA days paid xlsx sheet
</commit_message>
<xml_diff>
--- a/analyses/monitoring_costs/FMA Days Paid.xlsx
+++ b/analyses/monitoring_costs/FMA Days Paid.xlsx
@@ -10,14 +10,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="9Aub7KQy0WieWVTHoa8W3TspX4bRA1mWCuo5wWltqDg="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="r/q/QVS7d4055oGFR+VRF4mgjsNKzDg0QsA6Sr/TQoE="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="85">
   <si>
     <t>Contract</t>
   </si>
@@ -139,18 +139,43 @@
     <t>Aug23Aug24</t>
   </si>
   <si>
-    <t>Aug23Sept24</t>
-  </si>
-  <si>
-    <t>Extended contract from 8/17/24 - 9/30/2024 added 350 new Guaranteed days</t>
-  </si>
-  <si>
-    <t>Aug23Sept 24</t>
+    <t>did not separate travel ($92,274.89) over the extension, so this was split between both 2024 Aug lines proportionate to number of sea days</t>
+  </si>
+  <si>
+    <t>Aug24Aug24</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Extended contract from 8/17/24 - 9/30/2024 </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FFFF0000"/>
+      </rPr>
+      <t>added 350 new Guaranteed days</t>
+    </r>
+  </si>
+  <si>
+    <t>Aug24Sept24</t>
   </si>
   <si>
     <t>Extended contract from 8/17/24 - 9/30/2024</t>
   </si>
   <si>
+    <t>Oct24Sept25</t>
+  </si>
+  <si>
+    <t>Quarantine days were not included in the new contract.</t>
+  </si>
+  <si>
+    <t>$132 of travel was paid out from the previous contract</t>
+  </si>
+  <si>
     <t>Dates</t>
   </si>
   <si>
@@ -172,6 +197,9 @@
     <t>Plant_Day_Cost</t>
   </si>
   <si>
+    <t>Optional_Plant_Day_Cost</t>
+  </si>
+  <si>
     <t>6/17/16 - 6/16/17</t>
   </si>
   <si>
@@ -209,6 +237,54 @@
   </si>
   <si>
     <t>8/17/23 - 8/16/24</t>
+  </si>
+  <si>
+    <t>8/16/24 - 9/30/24</t>
+  </si>
+  <si>
+    <t>Option Year 4 Extended</t>
+  </si>
+  <si>
+    <t>added 350 days to the extension at the new base day cost</t>
+  </si>
+  <si>
+    <t>10/1/24 - 9/30/25</t>
+  </si>
+  <si>
+    <t>Oct25Sept26</t>
+  </si>
+  <si>
+    <t>10/1/25 - 9/30/26</t>
+  </si>
+  <si>
+    <t>Option Period 1</t>
+  </si>
+  <si>
+    <t>Oct26Sept27</t>
+  </si>
+  <si>
+    <t>10/1/26 - 9/30/27</t>
+  </si>
+  <si>
+    <t>Option Period 2</t>
+  </si>
+  <si>
+    <t>Oct27Sept28</t>
+  </si>
+  <si>
+    <t>10/1/27 - 9/30/28</t>
+  </si>
+  <si>
+    <t>Option Period 3</t>
+  </si>
+  <si>
+    <t>Oct28Sept29</t>
+  </si>
+  <si>
+    <t>10/1/28 - 9/30/29</t>
+  </si>
+  <si>
+    <t>Option Period 4</t>
   </si>
 </sst>
 </file>
@@ -218,7 +294,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -246,6 +322,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color rgb="FF9900FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -266,18 +347,12 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CC"/>
-        <bgColor rgb="FFFFF2CC"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -292,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -313,17 +388,20 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -332,13 +410,16 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -573,9 +654,9 @@
     <col customWidth="1" min="8" max="8" width="13.29"/>
     <col customWidth="1" min="9" max="9" width="10.71"/>
     <col customWidth="1" min="10" max="10" width="18.0"/>
-    <col customWidth="1" min="11" max="11" width="9.71"/>
-    <col customWidth="1" min="12" max="12" width="9.14"/>
-    <col customWidth="1" min="13" max="13" width="8.71"/>
+    <col customWidth="1" min="11" max="11" width="12.71"/>
+    <col customWidth="1" min="12" max="12" width="12.57"/>
+    <col customWidth="1" min="13" max="13" width="16.0"/>
     <col customWidth="1" min="14" max="14" width="57.71"/>
     <col customWidth="1" min="15" max="15" width="16.86"/>
     <col customWidth="1" min="16" max="16" width="12.43"/>
@@ -4635,8 +4716,8 @@
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
-      <c r="A98" s="2" t="s">
-        <v>40</v>
+      <c r="A98" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="B98" s="2">
         <v>2024.0</v>
@@ -4645,19 +4726,19 @@
         <v>25</v>
       </c>
       <c r="D98" s="2">
-        <v>106.5</v>
+        <v>0.0</v>
       </c>
       <c r="E98" s="2">
         <v>206.5</v>
       </c>
       <c r="F98" s="2">
-        <v>154028.82</v>
+        <v>0.0</v>
       </c>
       <c r="G98" s="2">
         <v>152516.77</v>
       </c>
-      <c r="H98" s="2">
-        <v>92274.89</v>
+      <c r="H98" s="9">
+        <v>60877.84</v>
       </c>
       <c r="I98" s="2">
         <v>0.0</v>
@@ -4674,37 +4755,495 @@
       <c r="M98" s="2">
         <v>0.0</v>
       </c>
-      <c r="N98" s="2" t="s">
-        <v>41</v>
+      <c r="N98" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B99" s="2">
         <v>2024.0</v>
       </c>
       <c r="C99" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D99" s="7">
+        <v>106.5</v>
+      </c>
+      <c r="E99" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F99" s="2">
+        <v>154028.82</v>
+      </c>
+      <c r="G99" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H99" s="9">
+        <v>31397.05</v>
+      </c>
+      <c r="I99" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J99" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K99" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L99" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M99" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="N99" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="100" ht="14.25" customHeight="1">
+      <c r="A100" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B100" s="2">
+        <v>2024.0</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N99" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
+      <c r="D100" s="7">
+        <v>243.5</v>
+      </c>
+      <c r="E100" s="2">
+        <v>315.0</v>
+      </c>
+      <c r="F100" s="2">
+        <v>352169.18</v>
+      </c>
+      <c r="G100" s="2">
+        <v>232652.7</v>
+      </c>
+      <c r="H100" s="2">
+        <v>119210.0</v>
+      </c>
+      <c r="I100" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J100" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K100" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L100" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M100" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="N100" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="101" ht="14.25" customHeight="1">
+      <c r="A101" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B101" s="2">
+        <v>2024.0</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D101" s="2">
+        <v>292.2</v>
+      </c>
+      <c r="E101" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F101" s="2">
+        <v>495448.48</v>
+      </c>
+      <c r="G101" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H101" s="2">
+        <v>128569.01</v>
+      </c>
+      <c r="I101" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J101" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K101" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L101" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M101" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="102" ht="14.25" customHeight="1">
+      <c r="A102" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B102" s="2">
+        <v>2024.0</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D102" s="2">
+        <v>101.4</v>
+      </c>
+      <c r="E102" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F102" s="2">
+        <v>171931.81</v>
+      </c>
+      <c r="G102" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H102" s="2">
+        <v>49369.04</v>
+      </c>
+      <c r="I102" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J102" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K102" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L102" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M102" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="103" ht="14.25" customHeight="1">
+      <c r="A103" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B103" s="2">
+        <v>2024.0</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D103" s="2">
+        <v>9.9</v>
+      </c>
+      <c r="E103" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F103" s="2">
+        <v>16786.24</v>
+      </c>
+      <c r="G103" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H103" s="2">
+        <v>18998.62</v>
+      </c>
+      <c r="I103" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J103" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K103" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L103" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M103" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="O103" s="13">
+        <v>899257.21</v>
+      </c>
+      <c r="P103" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="Q103" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="104" ht="14.25" customHeight="1">
+      <c r="A104" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B104" s="2">
+        <v>2025.0</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D104" s="2">
+        <v>100.58</v>
+      </c>
+      <c r="E104" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F104" s="2">
+        <v>170541.44</v>
+      </c>
+      <c r="G104" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H104" s="4">
+        <f>(52175.03+132) </f>
+        <v>52307.03</v>
+      </c>
+      <c r="I104" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J104" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K104" s="2">
+        <v>20.8</v>
+      </c>
+      <c r="L104" s="2">
+        <v>10782.02</v>
+      </c>
+      <c r="N104" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="105" ht="14.25" customHeight="1">
+      <c r="A105" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B105" s="2">
+        <v>2025.0</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D105" s="2">
+        <v>28.08</v>
+      </c>
+      <c r="E105" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F105" s="2">
+        <v>47611.89</v>
+      </c>
+      <c r="G105" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H105" s="2">
+        <v>54832.88</v>
+      </c>
+      <c r="I105" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J105" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K105" s="2">
+        <v>129.2</v>
+      </c>
+      <c r="L105" s="2">
+        <v>66876.5</v>
+      </c>
+    </row>
+    <row r="106" ht="14.25" customHeight="1">
+      <c r="A106" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B106" s="2">
+        <v>2025.0</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D106" s="2">
+        <v>53.54</v>
+      </c>
+      <c r="E106" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F106" s="2">
+        <v>90100.58</v>
+      </c>
+      <c r="G106" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H106" s="2">
+        <v>64832.88</v>
+      </c>
+      <c r="I106" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J106" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K106" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L106" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="107" ht="14.25" customHeight="1">
+      <c r="A107" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B107" s="2">
+        <v>2025.0</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D107" s="2">
+        <v>84.0</v>
+      </c>
+      <c r="E107" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F107" s="2">
+        <v>142428.72</v>
+      </c>
+      <c r="G107" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H107" s="2">
+        <v>71229.94</v>
+      </c>
+      <c r="I107" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J107" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K107" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L107" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="108" ht="14.25" customHeight="1">
+      <c r="A108" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B108" s="2">
+        <v>2025.0</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D108" s="2">
+        <v>65.67</v>
+      </c>
+      <c r="E108" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F108" s="2">
+        <v>111348.74</v>
+      </c>
+      <c r="G108" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H108" s="2">
+        <v>52500.01</v>
+      </c>
+      <c r="I108" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J108" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K108" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L108" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="109" ht="14.25" customHeight="1">
+      <c r="A109" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B109" s="2">
+        <v>2025.0</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D109" s="2">
+        <v>49.75</v>
+      </c>
+      <c r="E109" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F109" s="2">
+        <v>84355.11</v>
+      </c>
+      <c r="G109" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H109" s="2">
+        <v>34734.41</v>
+      </c>
+      <c r="I109" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J109" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K109" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L109" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="110" ht="14.25" customHeight="1">
+      <c r="A110" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B110" s="2">
+        <v>2025.0</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="111" ht="14.25" customHeight="1">
+      <c r="A111" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B111" s="2">
+        <v>2025.0</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="112" ht="14.25" customHeight="1">
+      <c r="A112" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B112" s="2">
+        <v>2025.0</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="113" ht="14.25" customHeight="1"/>
     <row r="114" ht="14.25" customHeight="1"/>
     <row r="115" ht="14.25" customHeight="1"/>
@@ -5598,6 +6137,7 @@
     <row r="1003" ht="14.25" customHeight="1"/>
     <row r="1004" ht="14.25" customHeight="1"/>
     <row r="1005" ht="14.25" customHeight="1"/>
+    <row r="1006" ht="14.25" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -5617,12 +6157,13 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="2" width="16.57"/>
-    <col customWidth="1" min="3" max="3" width="13.86"/>
+    <col customWidth="1" min="3" max="3" width="21.14"/>
     <col customWidth="1" min="4" max="4" width="14.14"/>
     <col customWidth="1" min="5" max="5" width="17.43"/>
     <col customWidth="1" min="6" max="6" width="19.71"/>
     <col customWidth="1" min="7" max="7" width="16.71"/>
     <col customWidth="1" min="8" max="8" width="14.43"/>
+    <col customWidth="1" min="9" max="9" width="22.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5630,25 +6171,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="2">
@@ -5656,104 +6200,104 @@
         <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="13">
+        <v>57</v>
+      </c>
+      <c r="D2" s="14">
         <v>1151.54</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="14">
         <v>564.26</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="13">
+        <v>59</v>
+      </c>
+      <c r="D3" s="14">
         <v>1174.56</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="14">
         <v>576.14</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="15">
+        <v>61</v>
+      </c>
+      <c r="D4" s="16">
         <v>1198.02</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="16">
         <v>589.01</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="13">
+        <v>63</v>
+      </c>
+      <c r="D5" s="14">
         <v>1255.42</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="14">
         <v>654.31</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="13">
+        <v>65</v>
+      </c>
+      <c r="D6" s="14">
         <v>1289.32</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="14">
         <v>671.98</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="14">
         <v>156.14</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="14">
         <v>265.0</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="14">
         <v>442.07</v>
       </c>
     </row>
@@ -5762,24 +6306,24 @@
         <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="13">
+        <v>57</v>
+      </c>
+      <c r="D7" s="14">
         <v>1328.0</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="14">
         <v>692.14</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="14">
         <v>156.14</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="14">
         <v>265.0</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="14">
         <v>442.07</v>
       </c>
     </row>
@@ -5788,24 +6332,24 @@
         <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="13">
+        <v>59</v>
+      </c>
+      <c r="D8" s="14">
         <v>1370.5</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="14">
         <v>714.29</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="14">
         <v>156.14</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="14">
         <v>265.0</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="14">
         <v>442.07</v>
       </c>
     </row>
@@ -5814,50 +6358,204 @@
         <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="14">
+        <v>1417.7</v>
+      </c>
+      <c r="E9" s="14">
+        <v>738.58</v>
+      </c>
+      <c r="F9" s="14">
+        <v>156.14</v>
+      </c>
+      <c r="G9" s="14">
+        <v>265.0</v>
+      </c>
+      <c r="H9" s="14">
+        <v>442.07</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="17">
+        <v>1446.28</v>
+      </c>
+      <c r="E10" s="18">
+        <v>738.58</v>
+      </c>
+      <c r="F10" s="18">
+        <v>156.14</v>
+      </c>
+      <c r="G10" s="18">
+        <v>265.0</v>
+      </c>
+      <c r="H10" s="18">
+        <v>442.07</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="13">
-        <v>1417.7</v>
-      </c>
-      <c r="E9" s="13">
-        <v>738.58</v>
-      </c>
-      <c r="F9" s="13">
-        <v>156.14</v>
-      </c>
-      <c r="G9" s="13">
-        <v>265.0</v>
-      </c>
-      <c r="H9" s="13">
-        <v>442.07</v>
+      <c r="D11" s="18">
+        <v>1695.58</v>
+      </c>
+      <c r="E11" s="18">
+        <v>877.73</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18">
+        <v>517.62</v>
+      </c>
+      <c r="I11" s="18">
+        <v>545.37</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="18">
+        <v>1754.93</v>
+      </c>
+      <c r="E12" s="18">
+        <v>908.45</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18">
+        <v>535.74</v>
+      </c>
+      <c r="I12" s="18">
+        <v>564.46</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="18">
+        <v>1807.58</v>
+      </c>
+      <c r="E13" s="18">
+        <v>935.7</v>
+      </c>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18">
+        <v>551.81</v>
+      </c>
+      <c r="I13" s="18">
+        <v>581.39</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="18">
+        <v>1857.29</v>
+      </c>
+      <c r="E14" s="18">
+        <v>961.43</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18">
+        <v>566.98</v>
+      </c>
+      <c r="I14" s="18">
+        <v>597.38</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="18">
+        <v>1899.08</v>
+      </c>
+      <c r="E15" s="18">
+        <v>983.06</v>
+      </c>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18">
+        <v>579.74</v>
+      </c>
+      <c r="I15" s="18">
+        <v>610.82</v>
       </c>
     </row>
     <row r="16">
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
     </row>
     <row r="17">
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
     </row>
     <row r="18">
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
     </row>
     <row r="19">
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
     </row>
     <row r="20">
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
     </row>
     <row r="24">
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>